<commit_message>
from 2010 to 2012
</commit_message>
<xml_diff>
--- a/Trend.xlsx
+++ b/Trend.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>Agri</t>
   </si>
@@ -159,42 +159,6 @@
   </si>
   <si>
     <t>lgrowth</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>2024</t>
-  </si>
-  <si>
-    <t>2026</t>
-  </si>
-  <si>
-    <t>2027</t>
-  </si>
-  <si>
-    <t>2028</t>
-  </si>
-  <si>
-    <t>2029</t>
   </si>
   <si>
     <t>hydro_Elec</t>
@@ -240,7 +204,7 @@
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="177" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,12 +234,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -285,20 +243,11 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -309,17 +258,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -461,12 +406,13 @@
             </c:trendlineLbl>
           </c:trendline>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$A$2:$A$18</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>2010</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2015</c:v>
@@ -516,8 +462,8 @@
                 <c:pt idx="16">
                   <c:v>2030</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -526,55 +472,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>40364.898000000001</c:v>
+                  <c:v>53680.017999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59572.146630201198</c:v>
+                  <c:v>66314.085250779273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63444.336161164276</c:v>
+                  <c:v>70624.500792079925</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67568.218011639954</c:v>
+                  <c:v>75215.09334356511</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>71960.152182396545</c:v>
+                  <c:v>80104.074410896836</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>76637.562074252317</c:v>
+                  <c:v>85310.839247605123</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>81619.003609078703</c:v>
+                  <c:v>90856.043798699451</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86516.14382562344</c:v>
+                  <c:v>96307.406426621426</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>91707.112455160852</c:v>
+                  <c:v>102085.85081221872</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>97209.539202470507</c:v>
+                  <c:v>108211.00186095184</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>103042.11155461874</c:v>
+                  <c:v>114703.66197260896</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103180.51754185146</c:v>
+                  <c:v>121585.8816909655</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>114685.87016029067</c:v>
+                  <c:v>127665.17577551378</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>120420.16366830521</c:v>
+                  <c:v>134048.43456428946</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>126441.17185172047</c:v>
+                  <c:v>140750.85629250394</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>132763.23044430651</c:v>
+                  <c:v>147788.39910712914</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>124332.44366427691</c:v>
+                  <c:v>155177.81906248559</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,16 +1256,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>628656</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304806</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28581</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>76206</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1628,23 +1574,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F26" sqref="F26"/>
+      <selection pane="topRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1657,15 +1601,15 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>2012</v>
       </c>
       <c r="B2">
-        <v>40364.898000000001</v>
+        <v>53680.017999999996</v>
       </c>
       <c r="C2" s="4">
-        <v>1.0000000137100569</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>7219.2939999999999</v>
@@ -1674,12 +1618,12 @@
         <v>7219.2939999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>2015</v>
       </c>
       <c r="B3">
-        <v>59572.146630201198</v>
+        <v>66314.085250779273</v>
       </c>
       <c r="C3" s="4">
         <v>1.1909626980161729</v>
@@ -1700,12 +1644,12 @@
         <v>7612.906540537725</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>43</v>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>2016</v>
       </c>
       <c r="B4">
-        <v>63444.336161164276</v>
+        <v>70624.500792079925</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
@@ -1719,12 +1663,12 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>44</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>2017</v>
       </c>
       <c r="B5">
-        <v>67568.218011639954</v>
+        <v>75215.09334356511</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1737,12 +1681,12 @@
         <v>7661.4031247459288</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>45</v>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>2018</v>
       </c>
       <c r="B6">
-        <v>71960.152182396545</v>
+        <v>80104.074410896836</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1755,12 +1699,12 @@
         <v>7628.3998880579056</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>46</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>2019</v>
       </c>
       <c r="B7">
-        <v>76637.562074252317</v>
+        <v>85310.839247605123</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -1774,12 +1718,12 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>37</v>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>2020</v>
       </c>
       <c r="B8">
-        <v>81619.003609078703</v>
+        <v>90856.043798699451</v>
       </c>
       <c r="C8" s="4">
         <v>1.4968698468829988</v>
@@ -1800,12 +1744,12 @@
         <v>7084.0870091985016</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>47</v>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>2021</v>
       </c>
       <c r="B9">
-        <v>86516.14382562344</v>
+        <v>96307.406426621426</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -1819,12 +1763,12 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>48</v>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>2022</v>
       </c>
       <c r="B10">
-        <v>91707.112455160852</v>
+        <v>102085.85081221872</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -1838,12 +1782,12 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>49</v>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>2023</v>
       </c>
       <c r="B11">
-        <v>97209.539202470507</v>
+        <v>108211.00186095184</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -1856,12 +1800,12 @@
         <v>7180.9898054591495</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>50</v>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
+        <v>2024</v>
       </c>
       <c r="B12">
-        <v>103042.11155461874</v>
+        <v>114703.66197260896</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -1874,12 +1818,12 @@
         <v>7109.042453522512</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>38</v>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
+        <v>2025</v>
       </c>
       <c r="B13">
-        <v>103180.51754185146</v>
+        <v>121585.8816909655</v>
       </c>
       <c r="C13" s="4">
         <v>1.7736509148562514</v>
@@ -1900,12 +1844,12 @@
         <v>6772.6975127782389</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>51</v>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
+        <v>2026</v>
       </c>
       <c r="B14">
-        <v>114685.87016029067</v>
+        <v>127665.17577551378</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -1918,12 +1862,12 @@
         <v>6964.0679043438722</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>52</v>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
+        <v>2027</v>
       </c>
       <c r="B15">
-        <v>120420.16366830521</v>
+        <v>134048.43456428946</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -1936,12 +1880,12 @@
         <v>6865.577977656244</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
-        <v>53</v>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
+        <v>2028</v>
       </c>
       <c r="B16">
-        <v>126441.17185172047</v>
+        <v>140750.85629250394</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
@@ -1953,28 +1897,13 @@
         <f t="shared" si="0"/>
         <v>6750.6559600110768</v>
       </c>
-      <c r="L16" s="6">
-        <v>216</v>
-      </c>
-      <c r="M16" s="6">
-        <v>10.82</v>
-      </c>
-      <c r="N16" s="6">
-        <v>29.58</v>
-      </c>
-      <c r="O16" s="6">
-        <v>0.26</v>
-      </c>
-      <c r="P16" s="6">
-        <v>3.41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
-        <v>54</v>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
+        <v>2029</v>
       </c>
       <c r="B17">
-        <v>132763.23044430651</v>
+        <v>147788.39910712914</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -1986,33 +1915,13 @@
         <f t="shared" si="0"/>
         <v>6620.1309841511174</v>
       </c>
-      <c r="L17" s="7">
-        <f>L$16*B27</f>
-        <v>216</v>
-      </c>
-      <c r="M17" s="7">
-        <f t="shared" ref="M17:P17" si="1">M$16*C27</f>
-        <v>10.82</v>
-      </c>
-      <c r="N17" s="7">
-        <f t="shared" si="1"/>
-        <v>29.58</v>
-      </c>
-      <c r="O17" s="7">
-        <f t="shared" si="1"/>
-        <v>0.26</v>
-      </c>
-      <c r="P17" s="7">
-        <f t="shared" si="1"/>
-        <v>3.41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
+        <v>2030</v>
       </c>
       <c r="B18">
-        <v>124332.44366427691</v>
+        <v>155177.81906248559</v>
       </c>
       <c r="C18" s="4">
         <v>2.1835159813744296</v>
@@ -2028,219 +1937,25 @@
         <f>G13*(1+D18)^5</f>
         <v>6061.8917315193021</v>
       </c>
-      <c r="L18" s="7">
-        <f t="shared" ref="L18:L22" si="2">L$16*B28</f>
-        <v>305.589</v>
-      </c>
-      <c r="M18" s="7">
-        <f t="shared" ref="M18:M22" si="3">M$16*C28</f>
-        <v>39.9</v>
-      </c>
-      <c r="N18" s="7">
-        <f t="shared" ref="N18:N22" si="4">N$16*D28</f>
-        <v>105.325</v>
-      </c>
-      <c r="O18" s="7">
-        <f t="shared" ref="O18:O22" si="5">O$16*E28</f>
-        <v>25.228727556596407</v>
-      </c>
-      <c r="P18" s="7">
-        <f t="shared" ref="P18:P22" si="6">P$16*F28</f>
-        <v>31.001000000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="L19" s="7">
-        <f t="shared" si="2"/>
-        <v>360.161</v>
-      </c>
-      <c r="M19" s="7">
-        <f t="shared" si="3"/>
-        <v>64.28</v>
-      </c>
-      <c r="N19" s="7">
-        <f t="shared" si="4"/>
-        <v>249.39</v>
-      </c>
-      <c r="O19" s="7">
-        <f t="shared" si="5"/>
-        <v>104.527</v>
-      </c>
-      <c r="P19" s="7">
-        <f t="shared" si="6"/>
-        <v>58.006000000000007</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="L20" s="7">
-        <f t="shared" si="2"/>
-        <v>467.41199999999998</v>
-      </c>
-      <c r="M20" s="7">
-        <f t="shared" si="3"/>
-        <v>111.9</v>
-      </c>
-      <c r="N20" s="7">
-        <f t="shared" si="4"/>
-        <v>632.17600000000004</v>
-      </c>
-      <c r="O20" s="7">
-        <f t="shared" si="5"/>
-        <v>500.23500000000001</v>
-      </c>
-      <c r="P20" s="7">
-        <f t="shared" si="6"/>
-        <v>70.671999999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="L21" s="7">
-        <f t="shared" si="2"/>
-        <v>522.06299999999999</v>
-      </c>
-      <c r="M21" s="7">
-        <f t="shared" si="3"/>
-        <v>159.52000000000001</v>
-      </c>
-      <c r="N21" s="7">
-        <f t="shared" si="4"/>
-        <v>1103.944</v>
-      </c>
-      <c r="O21" s="7">
-        <f t="shared" si="5"/>
-        <v>1048.8579999999999</v>
-      </c>
-      <c r="P21" s="7">
-        <f t="shared" si="6"/>
-        <v>87.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="L22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="L23" s="7">
-        <f>L$16*B38</f>
-        <v>216</v>
-      </c>
-      <c r="M23" s="7">
-        <f t="shared" ref="M23:P27" si="7">M$16*C38</f>
-        <v>10.82</v>
-      </c>
-      <c r="N23" s="7">
-        <f t="shared" si="7"/>
-        <v>29.58</v>
-      </c>
-      <c r="O23" s="7">
-        <f t="shared" si="7"/>
-        <v>0.26</v>
-      </c>
-      <c r="P23" s="7">
-        <f t="shared" si="7"/>
-        <v>3.41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="L24" s="7">
-        <f t="shared" ref="L24:L27" si="8">L$16*B39</f>
-        <v>305.589</v>
-      </c>
-      <c r="M24" s="7">
-        <f t="shared" si="7"/>
-        <v>39.9</v>
-      </c>
-      <c r="N24" s="7">
-        <f t="shared" si="7"/>
-        <v>105.325</v>
-      </c>
-      <c r="O24" s="7">
-        <f t="shared" si="7"/>
-        <v>25.228727556596407</v>
-      </c>
-      <c r="P24" s="7">
-        <f t="shared" si="7"/>
-        <v>31.001000000000005</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="L25" s="7">
-        <f t="shared" si="8"/>
-        <v>360.161</v>
-      </c>
-      <c r="M25" s="7">
-        <f t="shared" si="7"/>
-        <v>64.28</v>
-      </c>
-      <c r="N25" s="7">
-        <f t="shared" si="7"/>
-        <v>249.39</v>
-      </c>
-      <c r="O25" s="7">
-        <f t="shared" si="7"/>
-        <v>104.527</v>
-      </c>
-      <c r="P25" s="7">
-        <f t="shared" si="7"/>
-        <v>58.006000000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" s="7">
-        <f t="shared" si="8"/>
-        <v>427.78899999999999</v>
-      </c>
-      <c r="M26" s="7">
-        <f t="shared" si="7"/>
-        <v>82.76</v>
-      </c>
-      <c r="N26" s="7">
-        <f t="shared" si="7"/>
-        <v>434.54300000000001</v>
-      </c>
-      <c r="O26" s="7">
-        <f t="shared" si="7"/>
-        <v>171.71799999999999</v>
-      </c>
-      <c r="P26" s="7">
-        <f t="shared" si="7"/>
-        <v>61.195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -2260,31 +1975,8 @@
         <v>1</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="J27">
-        <v>10.82</v>
-      </c>
-      <c r="L27" s="7">
-        <f t="shared" si="8"/>
-        <v>497.26299999999998</v>
-      </c>
-      <c r="M27" s="7">
-        <f t="shared" si="7"/>
-        <v>112.85999999999999</v>
-      </c>
-      <c r="N27" s="7">
-        <f t="shared" si="7"/>
-        <v>592.471</v>
-      </c>
-      <c r="O27" s="7">
-        <f t="shared" si="7"/>
-        <v>309.923</v>
-      </c>
-      <c r="P27" s="7">
-        <f t="shared" si="7"/>
-        <v>68.602999999999994</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -2304,11 +1996,8 @@
         <v>9.0912023460410563</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="J28">
-        <v>39.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
@@ -2328,15 +2017,8 @@
         <v>17.010557184750734</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="J29">
-        <v>64.28</v>
-      </c>
-      <c r="K29">
-        <f>(J35-J29)/6</f>
-        <v>47.620000000000005</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -2356,16 +2038,8 @@
         <v>20.724926686217007</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="J30">
-        <f>J29+K29</f>
-        <v>111.9</v>
-      </c>
-      <c r="L30">
-        <f>J30/J27</f>
-        <v>10.341959334565619</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -2385,57 +2059,44 @@
         <v>25.689149560117301</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="J31">
-        <f>J30+K29</f>
-        <v>159.52000000000001</v>
-      </c>
-      <c r="L31">
-        <f>J31/J27</f>
-        <v>14.743068391866913</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="H33" s="1"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="J35">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B37" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -2455,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -2475,7 +2136,7 @@
         <v>9.0912023460410563</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -2495,7 +2156,7 @@
         <v>17.010557184750734</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -2515,7 +2176,7 @@
         <v>17.94574780058651</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -2535,42 +2196,36 @@
         <v>20.118181818181817</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>35</v>
       </c>
@@ -2589,14 +2244,8 @@
       <c r="F48">
         <v>1.0000000005320082</v>
       </c>
-      <c r="L48">
-        <v>1</v>
-      </c>
-      <c r="M48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>36</v>
       </c>
@@ -2615,14 +2264,8 @@
       <c r="F49">
         <v>8.2446938400081233</v>
       </c>
-      <c r="L49">
-        <v>1.0309308719560095</v>
-      </c>
-      <c r="M49">
-        <v>1.2053571428571428</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>37</v>
       </c>
@@ -2641,14 +2284,8 @@
       <c r="F50">
         <v>14.185224254344702</v>
       </c>
-      <c r="L50">
-        <v>1.0627454831107621</v>
-      </c>
-      <c r="M50">
-        <v>1.4464285714285714</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>38</v>
       </c>
@@ -2667,14 +2304,8 @@
       <c r="F51">
         <v>16.595936138113832</v>
       </c>
-      <c r="L51">
-        <v>1.0955420267085625</v>
-      </c>
-      <c r="M51">
-        <v>1.7499999999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>39</v>
       </c>
@@ -2693,31 +2324,25 @@
       <c r="F52">
         <v>20.042987525789183</v>
       </c>
-      <c r="L52">
-        <v>1.1293205027494109</v>
-      </c>
-      <c r="M52">
-        <v>2.1071428571428568</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B58" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
@@ -2737,7 +2362,7 @@
         <v>1.0000000005320082</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>36</v>
       </c>
@@ -2757,7 +2382,7 @@
         <v>8.2446938400081233</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>37</v>
       </c>
@@ -2777,7 +2402,7 @@
         <v>14.185224254344702</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>38</v>
       </c>
@@ -2797,7 +2422,7 @@
         <v>14.331324540148957</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>